<commit_message>
Data of (non-)existing networks
</commit_message>
<xml_diff>
--- a/Maaike/Network/Absent genes/Interactors FOR3.xlsx
+++ b/Maaike/Network/Absent genes/Interactors FOR3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAP Mariahoeve\Desktop\BEP\Git\Maaike\Network\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAP Mariahoeve\Desktop\BEP\Git\Maaike\Network\Absent genes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073F86DF-4325-4CAA-8069-99CD9F4927DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724F3F35-89D2-4CF6-9945-A895257AA07D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{FBC3F80B-EF61-4C32-B6B0-02160A80D8C6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{FBC3F80B-EF61-4C32-B6B0-02160A80D8C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequence interactors" sheetId="1" r:id="rId1"/>
@@ -365,9 +365,6 @@
     <t>Swi4</t>
   </si>
   <si>
-    <t>SCD1/PAL2</t>
-  </si>
-  <si>
     <t>SepA</t>
   </si>
   <si>
@@ -972,6 +969,9 @@
   </si>
   <si>
     <t>PB</t>
+  </si>
+  <si>
+    <t>SCD1</t>
   </si>
 </sst>
 </file>
@@ -1679,7 +1679,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1690,16 +1690,16 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D5" t="s">
+        <v>306</v>
+      </c>
+      <c r="E5" t="s">
         <v>307</v>
-      </c>
-      <c r="E5" t="s">
-        <v>308</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -1710,7 +1710,7 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1726,16 +1726,16 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F8">
         <v>3</v>
@@ -1751,7 +1751,7 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1801,21 +1801,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{582F3E21-849B-4E06-89B8-6F94FAE4B1F8}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E1" t="s">
         <v>310</v>
       </c>
-      <c r="E1" t="s">
-        <v>311</v>
-      </c>
       <c r="G1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1895,7 +1895,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1909,7 +1909,7 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2011,7 +2011,7 @@
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2113,7 +2113,7 @@
         <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2127,7 +2127,7 @@
         <v>2</v>
       </c>
       <c r="G28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2152,7 +2152,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2166,7 +2166,7 @@
         <v>3</v>
       </c>
       <c r="G31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2191,7 +2191,7 @@
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2205,7 +2205,7 @@
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2230,7 +2230,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -2256,8 +2256,8 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>109</v>
+      <c r="A39" s="2" t="s">
+        <v>311</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2268,7 +2268,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -2279,7 +2279,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -2290,7 +2290,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -2301,7 +2301,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -2319,775 +2319,776 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3CD1A6D-9E93-44E4-8ADF-1CFDC3D6D1B3}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="s">
         <v>117</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>118</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>119</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
         <v>121</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>122</v>
-      </c>
-      <c r="C3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
         <v>124</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>125</v>
-      </c>
-      <c r="C4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" t="s">
         <v>127</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>128</v>
-      </c>
-      <c r="C5" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" t="s">
         <v>130</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>131</v>
-      </c>
-      <c r="C6" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" t="s">
         <v>133</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>134</v>
-      </c>
-      <c r="C7" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" t="s">
         <v>136</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>137</v>
-      </c>
-      <c r="C8" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" t="s">
         <v>139</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>140</v>
-      </c>
-      <c r="C9" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" t="s">
         <v>142</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>143</v>
-      </c>
-      <c r="C10" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" t="s">
         <v>145</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>146</v>
-      </c>
-      <c r="C11" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" t="s">
         <v>117</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>118</v>
       </c>
-      <c r="C13" t="s">
-        <v>119</v>
-      </c>
       <c r="D13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" t="s">
         <v>149</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>150</v>
-      </c>
-      <c r="C14" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B15" t="s">
         <v>152</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>153</v>
-      </c>
-      <c r="C15" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" t="s">
         <v>155</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>156</v>
-      </c>
-      <c r="C16" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B17" t="s">
         <v>158</v>
-      </c>
-      <c r="B17" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>159</v>
+      </c>
+      <c r="B18" t="s">
         <v>160</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>161</v>
-      </c>
-      <c r="C18" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" t="s">
         <v>163</v>
-      </c>
-      <c r="B19" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>164</v>
+      </c>
+      <c r="B20" t="s">
         <v>165</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>166</v>
-      </c>
-      <c r="C20" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" t="s">
         <v>124</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>125</v>
-      </c>
-      <c r="C21" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" t="s">
         <v>168</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>169</v>
-      </c>
-      <c r="C22" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B23" t="s">
         <v>171</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>172</v>
-      </c>
-      <c r="C23" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>173</v>
+      </c>
+      <c r="B24" t="s">
         <v>174</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>175</v>
-      </c>
-      <c r="C24" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>176</v>
+      </c>
+      <c r="B25" t="s">
         <v>177</v>
       </c>
-      <c r="B25" t="s">
-        <v>178</v>
-      </c>
       <c r="C25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>178</v>
+      </c>
+      <c r="B26" t="s">
         <v>179</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>180</v>
-      </c>
-      <c r="C26" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" t="s">
         <v>136</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>137</v>
-      </c>
-      <c r="C27" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>181</v>
+      </c>
+      <c r="B28" t="s">
         <v>182</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>183</v>
-      </c>
-      <c r="C28" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>184</v>
+      </c>
+      <c r="B29" t="s">
         <v>185</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>186</v>
-      </c>
-      <c r="C29" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>187</v>
+      </c>
+      <c r="B30" t="s">
         <v>188</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>189</v>
-      </c>
-      <c r="C30" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>190</v>
+      </c>
+      <c r="B31" t="s">
         <v>191</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>192</v>
-      </c>
-      <c r="C31" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B32" t="s">
         <v>139</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>140</v>
-      </c>
-      <c r="C32" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>193</v>
+      </c>
+      <c r="B33" t="s">
         <v>194</v>
-      </c>
-      <c r="B33" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>195</v>
+      </c>
+      <c r="B34" t="s">
         <v>196</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>197</v>
-      </c>
-      <c r="C34" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>198</v>
+      </c>
+      <c r="B35" t="s">
         <v>199</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>200</v>
-      </c>
-      <c r="C35" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>201</v>
+      </c>
+      <c r="B36" t="s">
         <v>202</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>203</v>
-      </c>
-      <c r="C36" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>204</v>
+      </c>
+      <c r="B37" t="s">
         <v>205</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>206</v>
-      </c>
-      <c r="C37" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>207</v>
+      </c>
+      <c r="B38" t="s">
         <v>208</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>209</v>
-      </c>
-      <c r="C38" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>210</v>
+      </c>
+      <c r="B39" t="s">
         <v>211</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>212</v>
-      </c>
-      <c r="C39" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>213</v>
+      </c>
+      <c r="B40" t="s">
         <v>214</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>215</v>
-      </c>
-      <c r="C40" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>216</v>
+      </c>
+      <c r="B41" t="s">
         <v>217</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>218</v>
-      </c>
-      <c r="C41" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>219</v>
+      </c>
+      <c r="B42" t="s">
         <v>220</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>221</v>
-      </c>
-      <c r="C42" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>222</v>
+      </c>
+      <c r="B43" t="s">
         <v>223</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>224</v>
-      </c>
-      <c r="C43" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>144</v>
+      </c>
+      <c r="B44" t="s">
         <v>145</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>146</v>
-      </c>
-      <c r="C44" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>225</v>
+      </c>
+      <c r="B45" t="s">
         <v>226</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>227</v>
-      </c>
-      <c r="C45" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>228</v>
+      </c>
+      <c r="B46" t="s">
         <v>229</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>230</v>
-      </c>
-      <c r="C46" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>231</v>
+      </c>
+      <c r="B47" t="s">
         <v>232</v>
       </c>
-      <c r="B47" t="s">
-        <v>233</v>
-      </c>
       <c r="C47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B48" t="s">
         <v>234</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>235</v>
-      </c>
-      <c r="C48" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>236</v>
+      </c>
+      <c r="B49" t="s">
         <v>237</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>238</v>
-      </c>
-      <c r="C49" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>239</v>
+      </c>
+      <c r="B50" t="s">
         <v>240</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>241</v>
-      </c>
-      <c r="C50" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>242</v>
+      </c>
+      <c r="B51" t="s">
         <v>243</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>244</v>
-      </c>
-      <c r="C51" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>245</v>
+      </c>
+      <c r="B52" t="s">
         <v>246</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>247</v>
-      </c>
-      <c r="C52" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>248</v>
+      </c>
+      <c r="B53" t="s">
         <v>249</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>250</v>
-      </c>
-      <c r="C53" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>251</v>
+      </c>
+      <c r="B54" t="s">
         <v>252</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>253</v>
-      </c>
-      <c r="C54" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>254</v>
+      </c>
+      <c r="B55" t="s">
         <v>255</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>256</v>
-      </c>
-      <c r="C55" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>257</v>
+      </c>
+      <c r="B56" t="s">
         <v>258</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>259</v>
-      </c>
-      <c r="C56" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>260</v>
+      </c>
+      <c r="B57" t="s">
         <v>261</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>262</v>
-      </c>
-      <c r="C57" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>263</v>
+      </c>
+      <c r="B58" t="s">
         <v>264</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>265</v>
-      </c>
-      <c r="C58" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>266</v>
+      </c>
+      <c r="B59" t="s">
         <v>267</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>268</v>
-      </c>
-      <c r="C59" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>269</v>
+      </c>
+      <c r="B60" t="s">
         <v>270</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
         <v>271</v>
-      </c>
-      <c r="C60" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>272</v>
+      </c>
+      <c r="B61" t="s">
         <v>273</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>274</v>
-      </c>
-      <c r="C61" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>275</v>
+      </c>
+      <c r="B62" t="s">
         <v>276</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>277</v>
-      </c>
-      <c r="C62" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>278</v>
+      </c>
+      <c r="B63" t="s">
         <v>279</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>280</v>
-      </c>
-      <c r="C63" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>281</v>
+      </c>
+      <c r="B64" t="s">
         <v>282</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>283</v>
-      </c>
-      <c r="C64" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>284</v>
+      </c>
+      <c r="B65" t="s">
         <v>285</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>286</v>
-      </c>
-      <c r="C65" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>287</v>
+      </c>
+      <c r="B66" t="s">
         <v>288</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>289</v>
-      </c>
-      <c r="C66" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>290</v>
+      </c>
+      <c r="B67" t="s">
         <v>291</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>292</v>
-      </c>
-      <c r="C67" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>293</v>
+      </c>
+      <c r="B68" t="s">
         <v>294</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>295</v>
-      </c>
-      <c r="C68" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>296</v>
+      </c>
+      <c r="B69" t="s">
         <v>297</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>298</v>
-      </c>
-      <c r="C69" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>299</v>
+      </c>
+      <c r="B70" t="s">
         <v>300</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>301</v>
-      </c>
-      <c r="C70" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>302</v>
+      </c>
+      <c r="B71" t="s">
         <v>303</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
         <v>304</v>
-      </c>
-      <c r="C71" t="s">
-        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>